<commit_message>
WriteLetter Day -> Id로 변경
</commit_message>
<xml_diff>
--- a/Project_V/Assets/ExcelFiles/dialogue.xlsx
+++ b/Project_V/Assets/ExcelFiles/dialogue.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr codeName="현재_통합_문서"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tksth\Desktop\Project_V\Project_V\Assets\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A37D8F75-7C0A-44B9-840D-9D925A658267}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A571BA33-4594-41E2-8CAD-9812FED94A1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2820" yWindow="1935" windowWidth="19545" windowHeight="12240" xr2:uid="{461F5768-34F7-45FC-8921-4FFC2D7E081A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{461F5768-34F7-45FC-8921-4FFC2D7E081A}"/>
   </bookViews>
   <sheets>
     <sheet name="dialoguetest" sheetId="1" r:id="rId1"/>
@@ -1247,7 +1247,7 @@
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>